<commit_message>
add Favicon and minor updates
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -18,11 +18,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
       <sz val="10"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -79,35 +86,38 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,7 +411,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -523,7 +533,7 @@
       </c>
     </row>
     <row r="3" ht="13.8" customHeight="1">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="10" t="inlineStr">
         <is>
           <t>2203051240090</t>
         </is>

</xml_diff>